<commit_message>
updated comments for text limits and added updated Excel Template
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -253,21 +253,21 @@
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <t>unique identifier:
-A unique identifier for the dataset
+A unique identifier for the dataset. String limit is 100 characters.
 &lt;dcterms:identifier&gt;</t>
       </text>
     </comment>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <t>title:
-The official title for the dataset
+The official title for the dataset. String limit is 255 characters.
 &lt;dcterms:title&gt;</t>
       </text>
     </comment>
     <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <t>description:
-An account of the resource.
+An account of the resource. Text limit is 4,000 characters.
 &lt;dcterms:description&gt;</t>
       </text>
     </comment>
@@ -351,7 +351,7 @@
     <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <t>primaryITInvestmentUII:
-For linking a dataset with an IT Unique Investment Identifier (UII).
+For linking a dataset with an IT Unique Investment Identifier (UII). Can have multiple comma separated values.
 &lt;usg:primaryITInvestmentUII&gt;</t>
       </text>
     </comment>

</xml_diff>

<commit_message>
updating UII contraint, adding versionInfo to DIP record, adding date validation and other field shcal defs
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -813,14 +813,14 @@
     <comment ref="CC1" authorId="0" shapeId="0">
       <text>
         <t>recordTransmission:
-When the metadata record was transmitted.
+When the metadata record was transmitted. Must be a date.
 &lt;dhs:recordTransmission&gt;</t>
       </text>
     </comment>
     <comment ref="CD1" authorId="0" shapeId="0">
       <text>
         <t>validityTime:
-When the metadata record is valid.
+When the metadata record is valid. Must be in the form of a xsd Duration like P1Y or P3M
 &lt;dhs:validityTime&gt;</t>
       </text>
     </comment>
@@ -9908,7 +9908,7 @@
     <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H100 AV2:AV100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
+    <dataValidation sqref="H2:H100 AV2:AV100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
     <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot;, &quot;non-public&quot; or &quot;public restricted&quot; " type="list">
       <formula1>"public,non-public,public restricted"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
fixing excel template validation for accessLevel
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -9909,8 +9909,8 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H100 AV2:AV100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
-    <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot;, &quot;non-public&quot; or &quot;public restricted&quot; " type="list">
-      <formula1>"public,non-public,public restricted"</formula1>
+    <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot;, &quot;non-public&quot; or &quot;restricted public&quot; " type="list">
+      <formula1>"public,non-public,restricted public"</formula1>
     </dataValidation>
     <dataValidation sqref="AA2:AA100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a number between 1 and 100" type="whole" operator="lessThan">
       <formula1>101</formula1>

</xml_diff>

<commit_message>
added versioning in dhs_collect and Excel template, updated instructions link in Excel
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -1128,7 +1128,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>FY22 Data Inventory Collection Instrument</t>
+          <t>FY22 Data Inventory Collection Instrument - Version 1.4</t>
         </is>
       </c>
     </row>
@@ -1142,14 +1142,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>These instructions are stored in the file instructions.md.</t>
+          <t>Detailed instructions, including field definitions, can be found at: https://usdhs.github.io/dcat-tool/</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>For an actual data inventory, you would use instructions that are not in this repo.</t>
+          <t>Data can be submitted via upload or API using the DHS Mobius platform.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added validation for metadataClassification in easy_workbook.py
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -167,7 +167,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -9904,13 +9904,16 @@
       <c r="CD99" s="27" t="inlineStr"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
+  <dataValidations count="5">
+    <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100 BY2:BY100 BZ2:BZ100 CA2:CA100 CB2:CB100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation sqref="H2:H100 AV2:AV100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
     <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot;, &quot;non-public&quot; or &quot;restricted public&quot; " type="list">
       <formula1>"public,non-public,restricted public"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot; or &quot;non-public&quot; " type="list">
+      <formula1>"public,non-public"</formula1>
     </dataValidation>
     <dataValidation sqref="AA2:AA100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a number between 1 and 100" type="whole" operator="lessThan">
       <formula1>101</formula1>

</xml_diff>

<commit_message>
updating tests to use new characteristics class and updating documentation
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -819,12 +819,19 @@
     </comment>
     <comment ref="CD1" authorId="0" shapeId="0">
       <text>
+        <t>encryptionAlgorithm:
+Specifies encryption algorithm used to protect data at rest. Can have multiple comma separated values.
+&lt;usg:encryptionAlgorithm&gt;</t>
+      </text>
+    </comment>
+    <comment ref="CE1" authorId="0" shapeId="0">
+      <text>
         <t>recordTransmission:
 When the metadata record was transmitted. Must be a date.
 &lt;dhs:recordTransmission&gt;</t>
       </text>
     </comment>
-    <comment ref="CE1" authorId="0" shapeId="0">
+    <comment ref="CF1" authorId="0" shapeId="0">
       <text>
         <t>validityTime:
 When the metadata record is valid. Must be in the form of a xsd Duration like P1Y or P3M
@@ -1174,7 +1181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CE99"/>
+  <dimension ref="A1:CF99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1265,6 +1272,7 @@
     <col width="15" customWidth="1" min="81" max="81"/>
     <col width="15" customWidth="1" min="82" max="82"/>
     <col width="15" customWidth="1" min="83" max="83"/>
+    <col width="15" customWidth="1" min="84" max="84"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1675,10 +1683,15 @@
       </c>
       <c r="CD1" s="11" t="inlineStr">
         <is>
+          <t>encryptionAlgorithm</t>
+        </is>
+      </c>
+      <c r="CE1" s="12" t="inlineStr">
+        <is>
           <t>recordTransmission</t>
         </is>
       </c>
-      <c r="CE1" s="12" t="inlineStr">
+      <c r="CF1" s="12" t="inlineStr">
         <is>
           <t>validityTime</t>
         </is>
@@ -1768,6 +1781,7 @@
       <c r="CC2" s="33" t="inlineStr"/>
       <c r="CD2" s="26" t="inlineStr"/>
       <c r="CE2" s="27" t="inlineStr"/>
+      <c r="CF2" s="27" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="16" t="inlineStr"/>
@@ -1853,6 +1867,7 @@
       <c r="CC3" s="33" t="inlineStr"/>
       <c r="CD3" s="26" t="inlineStr"/>
       <c r="CE3" s="27" t="inlineStr"/>
+      <c r="CF3" s="27" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="16" t="inlineStr"/>
@@ -1938,6 +1953,7 @@
       <c r="CC4" s="33" t="inlineStr"/>
       <c r="CD4" s="26" t="inlineStr"/>
       <c r="CE4" s="27" t="inlineStr"/>
+      <c r="CF4" s="27" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="16" t="inlineStr"/>
@@ -2023,6 +2039,7 @@
       <c r="CC5" s="33" t="inlineStr"/>
       <c r="CD5" s="26" t="inlineStr"/>
       <c r="CE5" s="27" t="inlineStr"/>
+      <c r="CF5" s="27" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="16" t="inlineStr"/>
@@ -2108,6 +2125,7 @@
       <c r="CC6" s="33" t="inlineStr"/>
       <c r="CD6" s="26" t="inlineStr"/>
       <c r="CE6" s="27" t="inlineStr"/>
+      <c r="CF6" s="27" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="16" t="inlineStr"/>
@@ -2193,6 +2211,7 @@
       <c r="CC7" s="33" t="inlineStr"/>
       <c r="CD7" s="26" t="inlineStr"/>
       <c r="CE7" s="27" t="inlineStr"/>
+      <c r="CF7" s="27" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="16" t="inlineStr"/>
@@ -2278,6 +2297,7 @@
       <c r="CC8" s="33" t="inlineStr"/>
       <c r="CD8" s="26" t="inlineStr"/>
       <c r="CE8" s="27" t="inlineStr"/>
+      <c r="CF8" s="27" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="16" t="inlineStr"/>
@@ -2363,6 +2383,7 @@
       <c r="CC9" s="33" t="inlineStr"/>
       <c r="CD9" s="26" t="inlineStr"/>
       <c r="CE9" s="27" t="inlineStr"/>
+      <c r="CF9" s="27" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="16" t="inlineStr"/>
@@ -2448,6 +2469,7 @@
       <c r="CC10" s="33" t="inlineStr"/>
       <c r="CD10" s="26" t="inlineStr"/>
       <c r="CE10" s="27" t="inlineStr"/>
+      <c r="CF10" s="27" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="16" t="inlineStr"/>
@@ -2533,6 +2555,7 @@
       <c r="CC11" s="33" t="inlineStr"/>
       <c r="CD11" s="26" t="inlineStr"/>
       <c r="CE11" s="27" t="inlineStr"/>
+      <c r="CF11" s="27" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="16" t="inlineStr"/>
@@ -2618,6 +2641,7 @@
       <c r="CC12" s="33" t="inlineStr"/>
       <c r="CD12" s="26" t="inlineStr"/>
       <c r="CE12" s="27" t="inlineStr"/>
+      <c r="CF12" s="27" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="16" t="inlineStr"/>
@@ -2703,6 +2727,7 @@
       <c r="CC13" s="33" t="inlineStr"/>
       <c r="CD13" s="26" t="inlineStr"/>
       <c r="CE13" s="27" t="inlineStr"/>
+      <c r="CF13" s="27" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="16" t="inlineStr"/>
@@ -2788,6 +2813,7 @@
       <c r="CC14" s="33" t="inlineStr"/>
       <c r="CD14" s="26" t="inlineStr"/>
       <c r="CE14" s="27" t="inlineStr"/>
+      <c r="CF14" s="27" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="16" t="inlineStr"/>
@@ -2873,6 +2899,7 @@
       <c r="CC15" s="33" t="inlineStr"/>
       <c r="CD15" s="26" t="inlineStr"/>
       <c r="CE15" s="27" t="inlineStr"/>
+      <c r="CF15" s="27" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="16" t="inlineStr"/>
@@ -2958,6 +2985,7 @@
       <c r="CC16" s="33" t="inlineStr"/>
       <c r="CD16" s="26" t="inlineStr"/>
       <c r="CE16" s="27" t="inlineStr"/>
+      <c r="CF16" s="27" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="16" t="inlineStr"/>
@@ -3043,6 +3071,7 @@
       <c r="CC17" s="33" t="inlineStr"/>
       <c r="CD17" s="26" t="inlineStr"/>
       <c r="CE17" s="27" t="inlineStr"/>
+      <c r="CF17" s="27" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="16" t="inlineStr"/>
@@ -3128,6 +3157,7 @@
       <c r="CC18" s="33" t="inlineStr"/>
       <c r="CD18" s="26" t="inlineStr"/>
       <c r="CE18" s="27" t="inlineStr"/>
+      <c r="CF18" s="27" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="16" t="inlineStr"/>
@@ -3213,6 +3243,7 @@
       <c r="CC19" s="33" t="inlineStr"/>
       <c r="CD19" s="26" t="inlineStr"/>
       <c r="CE19" s="27" t="inlineStr"/>
+      <c r="CF19" s="27" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="16" t="inlineStr"/>
@@ -3298,6 +3329,7 @@
       <c r="CC20" s="33" t="inlineStr"/>
       <c r="CD20" s="26" t="inlineStr"/>
       <c r="CE20" s="27" t="inlineStr"/>
+      <c r="CF20" s="27" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="16" t="inlineStr"/>
@@ -3383,6 +3415,7 @@
       <c r="CC21" s="33" t="inlineStr"/>
       <c r="CD21" s="26" t="inlineStr"/>
       <c r="CE21" s="27" t="inlineStr"/>
+      <c r="CF21" s="27" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="16" t="inlineStr"/>
@@ -3468,6 +3501,7 @@
       <c r="CC22" s="33" t="inlineStr"/>
       <c r="CD22" s="26" t="inlineStr"/>
       <c r="CE22" s="27" t="inlineStr"/>
+      <c r="CF22" s="27" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="16" t="inlineStr"/>
@@ -3553,6 +3587,7 @@
       <c r="CC23" s="33" t="inlineStr"/>
       <c r="CD23" s="26" t="inlineStr"/>
       <c r="CE23" s="27" t="inlineStr"/>
+      <c r="CF23" s="27" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="16" t="inlineStr"/>
@@ -3638,6 +3673,7 @@
       <c r="CC24" s="33" t="inlineStr"/>
       <c r="CD24" s="26" t="inlineStr"/>
       <c r="CE24" s="27" t="inlineStr"/>
+      <c r="CF24" s="27" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="16" t="inlineStr"/>
@@ -3723,6 +3759,7 @@
       <c r="CC25" s="33" t="inlineStr"/>
       <c r="CD25" s="26" t="inlineStr"/>
       <c r="CE25" s="27" t="inlineStr"/>
+      <c r="CF25" s="27" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="16" t="inlineStr"/>
@@ -3808,6 +3845,7 @@
       <c r="CC26" s="33" t="inlineStr"/>
       <c r="CD26" s="26" t="inlineStr"/>
       <c r="CE26" s="27" t="inlineStr"/>
+      <c r="CF26" s="27" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="16" t="inlineStr"/>
@@ -3893,6 +3931,7 @@
       <c r="CC27" s="33" t="inlineStr"/>
       <c r="CD27" s="26" t="inlineStr"/>
       <c r="CE27" s="27" t="inlineStr"/>
+      <c r="CF27" s="27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="16" t="inlineStr"/>
@@ -3978,6 +4017,7 @@
       <c r="CC28" s="33" t="inlineStr"/>
       <c r="CD28" s="26" t="inlineStr"/>
       <c r="CE28" s="27" t="inlineStr"/>
+      <c r="CF28" s="27" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="16" t="inlineStr"/>
@@ -4063,6 +4103,7 @@
       <c r="CC29" s="33" t="inlineStr"/>
       <c r="CD29" s="26" t="inlineStr"/>
       <c r="CE29" s="27" t="inlineStr"/>
+      <c r="CF29" s="27" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="16" t="inlineStr"/>
@@ -4148,6 +4189,7 @@
       <c r="CC30" s="33" t="inlineStr"/>
       <c r="CD30" s="26" t="inlineStr"/>
       <c r="CE30" s="27" t="inlineStr"/>
+      <c r="CF30" s="27" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="16" t="inlineStr"/>
@@ -4233,6 +4275,7 @@
       <c r="CC31" s="33" t="inlineStr"/>
       <c r="CD31" s="26" t="inlineStr"/>
       <c r="CE31" s="27" t="inlineStr"/>
+      <c r="CF31" s="27" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="16" t="inlineStr"/>
@@ -4318,6 +4361,7 @@
       <c r="CC32" s="33" t="inlineStr"/>
       <c r="CD32" s="26" t="inlineStr"/>
       <c r="CE32" s="27" t="inlineStr"/>
+      <c r="CF32" s="27" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="16" t="inlineStr"/>
@@ -4403,6 +4447,7 @@
       <c r="CC33" s="33" t="inlineStr"/>
       <c r="CD33" s="26" t="inlineStr"/>
       <c r="CE33" s="27" t="inlineStr"/>
+      <c r="CF33" s="27" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="16" t="inlineStr"/>
@@ -4488,6 +4533,7 @@
       <c r="CC34" s="33" t="inlineStr"/>
       <c r="CD34" s="26" t="inlineStr"/>
       <c r="CE34" s="27" t="inlineStr"/>
+      <c r="CF34" s="27" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="16" t="inlineStr"/>
@@ -4573,6 +4619,7 @@
       <c r="CC35" s="33" t="inlineStr"/>
       <c r="CD35" s="26" t="inlineStr"/>
       <c r="CE35" s="27" t="inlineStr"/>
+      <c r="CF35" s="27" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="16" t="inlineStr"/>
@@ -4658,6 +4705,7 @@
       <c r="CC36" s="33" t="inlineStr"/>
       <c r="CD36" s="26" t="inlineStr"/>
       <c r="CE36" s="27" t="inlineStr"/>
+      <c r="CF36" s="27" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="16" t="inlineStr"/>
@@ -4743,6 +4791,7 @@
       <c r="CC37" s="33" t="inlineStr"/>
       <c r="CD37" s="26" t="inlineStr"/>
       <c r="CE37" s="27" t="inlineStr"/>
+      <c r="CF37" s="27" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="16" t="inlineStr"/>
@@ -4828,6 +4877,7 @@
       <c r="CC38" s="33" t="inlineStr"/>
       <c r="CD38" s="26" t="inlineStr"/>
       <c r="CE38" s="27" t="inlineStr"/>
+      <c r="CF38" s="27" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="16" t="inlineStr"/>
@@ -4913,6 +4963,7 @@
       <c r="CC39" s="33" t="inlineStr"/>
       <c r="CD39" s="26" t="inlineStr"/>
       <c r="CE39" s="27" t="inlineStr"/>
+      <c r="CF39" s="27" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="16" t="inlineStr"/>
@@ -4998,6 +5049,7 @@
       <c r="CC40" s="33" t="inlineStr"/>
       <c r="CD40" s="26" t="inlineStr"/>
       <c r="CE40" s="27" t="inlineStr"/>
+      <c r="CF40" s="27" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="16" t="inlineStr"/>
@@ -5083,6 +5135,7 @@
       <c r="CC41" s="33" t="inlineStr"/>
       <c r="CD41" s="26" t="inlineStr"/>
       <c r="CE41" s="27" t="inlineStr"/>
+      <c r="CF41" s="27" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="16" t="inlineStr"/>
@@ -5168,6 +5221,7 @@
       <c r="CC42" s="33" t="inlineStr"/>
       <c r="CD42" s="26" t="inlineStr"/>
       <c r="CE42" s="27" t="inlineStr"/>
+      <c r="CF42" s="27" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="16" t="inlineStr"/>
@@ -5253,6 +5307,7 @@
       <c r="CC43" s="33" t="inlineStr"/>
       <c r="CD43" s="26" t="inlineStr"/>
       <c r="CE43" s="27" t="inlineStr"/>
+      <c r="CF43" s="27" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="16" t="inlineStr"/>
@@ -5338,6 +5393,7 @@
       <c r="CC44" s="33" t="inlineStr"/>
       <c r="CD44" s="26" t="inlineStr"/>
       <c r="CE44" s="27" t="inlineStr"/>
+      <c r="CF44" s="27" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="16" t="inlineStr"/>
@@ -5423,6 +5479,7 @@
       <c r="CC45" s="33" t="inlineStr"/>
       <c r="CD45" s="26" t="inlineStr"/>
       <c r="CE45" s="27" t="inlineStr"/>
+      <c r="CF45" s="27" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="16" t="inlineStr"/>
@@ -5508,6 +5565,7 @@
       <c r="CC46" s="33" t="inlineStr"/>
       <c r="CD46" s="26" t="inlineStr"/>
       <c r="CE46" s="27" t="inlineStr"/>
+      <c r="CF46" s="27" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="16" t="inlineStr"/>
@@ -5593,6 +5651,7 @@
       <c r="CC47" s="33" t="inlineStr"/>
       <c r="CD47" s="26" t="inlineStr"/>
       <c r="CE47" s="27" t="inlineStr"/>
+      <c r="CF47" s="27" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="16" t="inlineStr"/>
@@ -5678,6 +5737,7 @@
       <c r="CC48" s="33" t="inlineStr"/>
       <c r="CD48" s="26" t="inlineStr"/>
       <c r="CE48" s="27" t="inlineStr"/>
+      <c r="CF48" s="27" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="16" t="inlineStr"/>
@@ -5763,6 +5823,7 @@
       <c r="CC49" s="33" t="inlineStr"/>
       <c r="CD49" s="26" t="inlineStr"/>
       <c r="CE49" s="27" t="inlineStr"/>
+      <c r="CF49" s="27" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="16" t="inlineStr"/>
@@ -5848,6 +5909,7 @@
       <c r="CC50" s="33" t="inlineStr"/>
       <c r="CD50" s="26" t="inlineStr"/>
       <c r="CE50" s="27" t="inlineStr"/>
+      <c r="CF50" s="27" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="16" t="inlineStr"/>
@@ -5933,6 +5995,7 @@
       <c r="CC51" s="33" t="inlineStr"/>
       <c r="CD51" s="26" t="inlineStr"/>
       <c r="CE51" s="27" t="inlineStr"/>
+      <c r="CF51" s="27" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="16" t="inlineStr"/>
@@ -6018,6 +6081,7 @@
       <c r="CC52" s="33" t="inlineStr"/>
       <c r="CD52" s="26" t="inlineStr"/>
       <c r="CE52" s="27" t="inlineStr"/>
+      <c r="CF52" s="27" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="16" t="inlineStr"/>
@@ -6103,6 +6167,7 @@
       <c r="CC53" s="33" t="inlineStr"/>
       <c r="CD53" s="26" t="inlineStr"/>
       <c r="CE53" s="27" t="inlineStr"/>
+      <c r="CF53" s="27" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="16" t="inlineStr"/>
@@ -6188,6 +6253,7 @@
       <c r="CC54" s="33" t="inlineStr"/>
       <c r="CD54" s="26" t="inlineStr"/>
       <c r="CE54" s="27" t="inlineStr"/>
+      <c r="CF54" s="27" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="16" t="inlineStr"/>
@@ -6273,6 +6339,7 @@
       <c r="CC55" s="33" t="inlineStr"/>
       <c r="CD55" s="26" t="inlineStr"/>
       <c r="CE55" s="27" t="inlineStr"/>
+      <c r="CF55" s="27" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="16" t="inlineStr"/>
@@ -6358,6 +6425,7 @@
       <c r="CC56" s="33" t="inlineStr"/>
       <c r="CD56" s="26" t="inlineStr"/>
       <c r="CE56" s="27" t="inlineStr"/>
+      <c r="CF56" s="27" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="16" t="inlineStr"/>
@@ -6443,6 +6511,7 @@
       <c r="CC57" s="33" t="inlineStr"/>
       <c r="CD57" s="26" t="inlineStr"/>
       <c r="CE57" s="27" t="inlineStr"/>
+      <c r="CF57" s="27" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="16" t="inlineStr"/>
@@ -6528,6 +6597,7 @@
       <c r="CC58" s="33" t="inlineStr"/>
       <c r="CD58" s="26" t="inlineStr"/>
       <c r="CE58" s="27" t="inlineStr"/>
+      <c r="CF58" s="27" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="16" t="inlineStr"/>
@@ -6613,6 +6683,7 @@
       <c r="CC59" s="33" t="inlineStr"/>
       <c r="CD59" s="26" t="inlineStr"/>
       <c r="CE59" s="27" t="inlineStr"/>
+      <c r="CF59" s="27" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="16" t="inlineStr"/>
@@ -6698,6 +6769,7 @@
       <c r="CC60" s="33" t="inlineStr"/>
       <c r="CD60" s="26" t="inlineStr"/>
       <c r="CE60" s="27" t="inlineStr"/>
+      <c r="CF60" s="27" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="16" t="inlineStr"/>
@@ -6783,6 +6855,7 @@
       <c r="CC61" s="33" t="inlineStr"/>
       <c r="CD61" s="26" t="inlineStr"/>
       <c r="CE61" s="27" t="inlineStr"/>
+      <c r="CF61" s="27" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="16" t="inlineStr"/>
@@ -6868,6 +6941,7 @@
       <c r="CC62" s="33" t="inlineStr"/>
       <c r="CD62" s="26" t="inlineStr"/>
       <c r="CE62" s="27" t="inlineStr"/>
+      <c r="CF62" s="27" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="16" t="inlineStr"/>
@@ -6953,6 +7027,7 @@
       <c r="CC63" s="33" t="inlineStr"/>
       <c r="CD63" s="26" t="inlineStr"/>
       <c r="CE63" s="27" t="inlineStr"/>
+      <c r="CF63" s="27" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="16" t="inlineStr"/>
@@ -7038,6 +7113,7 @@
       <c r="CC64" s="33" t="inlineStr"/>
       <c r="CD64" s="26" t="inlineStr"/>
       <c r="CE64" s="27" t="inlineStr"/>
+      <c r="CF64" s="27" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="16" t="inlineStr"/>
@@ -7123,6 +7199,7 @@
       <c r="CC65" s="33" t="inlineStr"/>
       <c r="CD65" s="26" t="inlineStr"/>
       <c r="CE65" s="27" t="inlineStr"/>
+      <c r="CF65" s="27" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="16" t="inlineStr"/>
@@ -7208,6 +7285,7 @@
       <c r="CC66" s="33" t="inlineStr"/>
       <c r="CD66" s="26" t="inlineStr"/>
       <c r="CE66" s="27" t="inlineStr"/>
+      <c r="CF66" s="27" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="16" t="inlineStr"/>
@@ -7293,6 +7371,7 @@
       <c r="CC67" s="33" t="inlineStr"/>
       <c r="CD67" s="26" t="inlineStr"/>
       <c r="CE67" s="27" t="inlineStr"/>
+      <c r="CF67" s="27" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="16" t="inlineStr"/>
@@ -7378,6 +7457,7 @@
       <c r="CC68" s="33" t="inlineStr"/>
       <c r="CD68" s="26" t="inlineStr"/>
       <c r="CE68" s="27" t="inlineStr"/>
+      <c r="CF68" s="27" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="16" t="inlineStr"/>
@@ -7463,6 +7543,7 @@
       <c r="CC69" s="33" t="inlineStr"/>
       <c r="CD69" s="26" t="inlineStr"/>
       <c r="CE69" s="27" t="inlineStr"/>
+      <c r="CF69" s="27" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="16" t="inlineStr"/>
@@ -7548,6 +7629,7 @@
       <c r="CC70" s="33" t="inlineStr"/>
       <c r="CD70" s="26" t="inlineStr"/>
       <c r="CE70" s="27" t="inlineStr"/>
+      <c r="CF70" s="27" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="16" t="inlineStr"/>
@@ -7633,6 +7715,7 @@
       <c r="CC71" s="33" t="inlineStr"/>
       <c r="CD71" s="26" t="inlineStr"/>
       <c r="CE71" s="27" t="inlineStr"/>
+      <c r="CF71" s="27" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="16" t="inlineStr"/>
@@ -7718,6 +7801,7 @@
       <c r="CC72" s="33" t="inlineStr"/>
       <c r="CD72" s="26" t="inlineStr"/>
       <c r="CE72" s="27" t="inlineStr"/>
+      <c r="CF72" s="27" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="16" t="inlineStr"/>
@@ -7803,6 +7887,7 @@
       <c r="CC73" s="33" t="inlineStr"/>
       <c r="CD73" s="26" t="inlineStr"/>
       <c r="CE73" s="27" t="inlineStr"/>
+      <c r="CF73" s="27" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="16" t="inlineStr"/>
@@ -7888,6 +7973,7 @@
       <c r="CC74" s="33" t="inlineStr"/>
       <c r="CD74" s="26" t="inlineStr"/>
       <c r="CE74" s="27" t="inlineStr"/>
+      <c r="CF74" s="27" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="16" t="inlineStr"/>
@@ -7973,6 +8059,7 @@
       <c r="CC75" s="33" t="inlineStr"/>
       <c r="CD75" s="26" t="inlineStr"/>
       <c r="CE75" s="27" t="inlineStr"/>
+      <c r="CF75" s="27" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="16" t="inlineStr"/>
@@ -8058,6 +8145,7 @@
       <c r="CC76" s="33" t="inlineStr"/>
       <c r="CD76" s="26" t="inlineStr"/>
       <c r="CE76" s="27" t="inlineStr"/>
+      <c r="CF76" s="27" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="16" t="inlineStr"/>
@@ -8143,6 +8231,7 @@
       <c r="CC77" s="33" t="inlineStr"/>
       <c r="CD77" s="26" t="inlineStr"/>
       <c r="CE77" s="27" t="inlineStr"/>
+      <c r="CF77" s="27" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="16" t="inlineStr"/>
@@ -8228,6 +8317,7 @@
       <c r="CC78" s="33" t="inlineStr"/>
       <c r="CD78" s="26" t="inlineStr"/>
       <c r="CE78" s="27" t="inlineStr"/>
+      <c r="CF78" s="27" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="16" t="inlineStr"/>
@@ -8313,6 +8403,7 @@
       <c r="CC79" s="33" t="inlineStr"/>
       <c r="CD79" s="26" t="inlineStr"/>
       <c r="CE79" s="27" t="inlineStr"/>
+      <c r="CF79" s="27" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="16" t="inlineStr"/>
@@ -8398,6 +8489,7 @@
       <c r="CC80" s="33" t="inlineStr"/>
       <c r="CD80" s="26" t="inlineStr"/>
       <c r="CE80" s="27" t="inlineStr"/>
+      <c r="CF80" s="27" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="16" t="inlineStr"/>
@@ -8483,6 +8575,7 @@
       <c r="CC81" s="33" t="inlineStr"/>
       <c r="CD81" s="26" t="inlineStr"/>
       <c r="CE81" s="27" t="inlineStr"/>
+      <c r="CF81" s="27" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="16" t="inlineStr"/>
@@ -8568,6 +8661,7 @@
       <c r="CC82" s="33" t="inlineStr"/>
       <c r="CD82" s="26" t="inlineStr"/>
       <c r="CE82" s="27" t="inlineStr"/>
+      <c r="CF82" s="27" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="16" t="inlineStr"/>
@@ -8653,6 +8747,7 @@
       <c r="CC83" s="33" t="inlineStr"/>
       <c r="CD83" s="26" t="inlineStr"/>
       <c r="CE83" s="27" t="inlineStr"/>
+      <c r="CF83" s="27" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="16" t="inlineStr"/>
@@ -8738,6 +8833,7 @@
       <c r="CC84" s="33" t="inlineStr"/>
       <c r="CD84" s="26" t="inlineStr"/>
       <c r="CE84" s="27" t="inlineStr"/>
+      <c r="CF84" s="27" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="16" t="inlineStr"/>
@@ -8823,6 +8919,7 @@
       <c r="CC85" s="33" t="inlineStr"/>
       <c r="CD85" s="26" t="inlineStr"/>
       <c r="CE85" s="27" t="inlineStr"/>
+      <c r="CF85" s="27" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="16" t="inlineStr"/>
@@ -8908,6 +9005,7 @@
       <c r="CC86" s="33" t="inlineStr"/>
       <c r="CD86" s="26" t="inlineStr"/>
       <c r="CE86" s="27" t="inlineStr"/>
+      <c r="CF86" s="27" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="16" t="inlineStr"/>
@@ -8993,6 +9091,7 @@
       <c r="CC87" s="33" t="inlineStr"/>
       <c r="CD87" s="26" t="inlineStr"/>
       <c r="CE87" s="27" t="inlineStr"/>
+      <c r="CF87" s="27" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="16" t="inlineStr"/>
@@ -9078,6 +9177,7 @@
       <c r="CC88" s="33" t="inlineStr"/>
       <c r="CD88" s="26" t="inlineStr"/>
       <c r="CE88" s="27" t="inlineStr"/>
+      <c r="CF88" s="27" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="16" t="inlineStr"/>
@@ -9163,6 +9263,7 @@
       <c r="CC89" s="33" t="inlineStr"/>
       <c r="CD89" s="26" t="inlineStr"/>
       <c r="CE89" s="27" t="inlineStr"/>
+      <c r="CF89" s="27" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="16" t="inlineStr"/>
@@ -9248,6 +9349,7 @@
       <c r="CC90" s="33" t="inlineStr"/>
       <c r="CD90" s="26" t="inlineStr"/>
       <c r="CE90" s="27" t="inlineStr"/>
+      <c r="CF90" s="27" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="16" t="inlineStr"/>
@@ -9333,6 +9435,7 @@
       <c r="CC91" s="33" t="inlineStr"/>
       <c r="CD91" s="26" t="inlineStr"/>
       <c r="CE91" s="27" t="inlineStr"/>
+      <c r="CF91" s="27" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="16" t="inlineStr"/>
@@ -9418,6 +9521,7 @@
       <c r="CC92" s="33" t="inlineStr"/>
       <c r="CD92" s="26" t="inlineStr"/>
       <c r="CE92" s="27" t="inlineStr"/>
+      <c r="CF92" s="27" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="16" t="inlineStr"/>
@@ -9503,6 +9607,7 @@
       <c r="CC93" s="33" t="inlineStr"/>
       <c r="CD93" s="26" t="inlineStr"/>
       <c r="CE93" s="27" t="inlineStr"/>
+      <c r="CF93" s="27" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="16" t="inlineStr"/>
@@ -9588,6 +9693,7 @@
       <c r="CC94" s="33" t="inlineStr"/>
       <c r="CD94" s="26" t="inlineStr"/>
       <c r="CE94" s="27" t="inlineStr"/>
+      <c r="CF94" s="27" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="16" t="inlineStr"/>
@@ -9673,6 +9779,7 @@
       <c r="CC95" s="33" t="inlineStr"/>
       <c r="CD95" s="26" t="inlineStr"/>
       <c r="CE95" s="27" t="inlineStr"/>
+      <c r="CF95" s="27" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="16" t="inlineStr"/>
@@ -9758,6 +9865,7 @@
       <c r="CC96" s="33" t="inlineStr"/>
       <c r="CD96" s="26" t="inlineStr"/>
       <c r="CE96" s="27" t="inlineStr"/>
+      <c r="CF96" s="27" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="16" t="inlineStr"/>
@@ -9843,6 +9951,7 @@
       <c r="CC97" s="33" t="inlineStr"/>
       <c r="CD97" s="26" t="inlineStr"/>
       <c r="CE97" s="27" t="inlineStr"/>
+      <c r="CF97" s="27" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="16" t="inlineStr"/>
@@ -9928,6 +10037,7 @@
       <c r="CC98" s="33" t="inlineStr"/>
       <c r="CD98" s="26" t="inlineStr"/>
       <c r="CE98" s="27" t="inlineStr"/>
+      <c r="CF98" s="27" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="16" t="inlineStr"/>
@@ -10013,15 +10123,19 @@
       <c r="CC99" s="33" t="inlineStr"/>
       <c r="CD99" s="26" t="inlineStr"/>
       <c r="CE99" s="27" t="inlineStr"/>
+      <c r="CF99" s="27" t="inlineStr"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BG2:BG100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100 BX2:BX100 BZ2:BZ100 CA2:CA100 CB2:CB100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation sqref="H2:H100 AV2:AV100 CD2:CD100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
+    <dataValidation sqref="H2:H100 AV2:AV100 CE2:CE100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a date" promptTitle="Date Field" prompt="Please enter a date" type="date"/>
     <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot;, &quot;non-public&quot; or &quot;restricted public&quot; " type="list">
       <formula1>"public,non-public,restricted public"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Entry" error="Must be one of the following: &quot;public&quot; or &quot;non-public&quot; " type="list">
+      <formula1>"public,non-public"</formula1>
     </dataValidation>
     <dataValidation sqref="AA2:AA100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a number between 1 and 100" type="whole" operator="lessThan">
       <formula1>101</formula1>

</xml_diff>

<commit_message>
added no-space validation for unique identifier in Excel Template and updated Template
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -10126,7 +10126,7 @@
       <c r="CF99" s="27" t="inlineStr"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BG2:BG100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100 BX2:BX100 BZ2:BZ100 CA2:CA100 CB2:CB100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -10140,6 +10140,9 @@
     <dataValidation sqref="AA2:AA100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a number between 1 and 100" type="whole" operator="lessThan">
       <formula1>101</formula1>
     </dataValidation>
+    <dataValidation sqref="A2:A100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be string with no spaces and a max of 128 chars" type="custom">
+      <formula1>AND(LEN(A2)&lt;129,NOT(ISNUMBER(SEARCH(" ",A2))))</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>

</xml_diff>

<commit_message>
fixing minor spelling errors and adding comment HTML cleaner on make_template plus testing on excel validation
</commit_message>
<xml_diff>
--- a/docs/samples/DIP_Excel_Template.xlsx
+++ b/docs/samples/DIP_Excel_Template.xlsx
@@ -254,651 +254,873 @@
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <t>unique identifier:
-&lt;p&gt;Similar to a serial number associated with your laptop, the identifier is a unique and specific combination of characters that identify the resource. The combination must start with the DHS component code, is limited to 128 characters, and be in the following format: code-xxx-x&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;mgmt-test-2&lt;/li&gt;&lt;li&gt;fema-1234-D&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+Similar to a serial number associated with your laptop, the identifier is a unique and specific combination of characters that identify the resource. The combination must start with the DHS component code, is limited to 128 characters, and be in the following format: code-xxx-x
+Example:
+mgmt-test-2
+fema-1234-D
 &lt;dcterms:identifier&gt;</t>
       </text>
     </comment>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <t>title:
-&lt;p&gt;The official name (title) given to the resource, limited to 255 characters. Acronyms should be used sparingly and only when explained in the description.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;DHS Data Inventory Introduction&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The official name (title) given to the resource, limited to 255 characters. Acronyms should be used sparingly and only when explained in the description.
+Example:
+DHS Data Inventory Introduction
 &lt;dcterms:title&gt;</t>
       </text>
     </comment>
     <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <t>description:
-&lt;p&gt;A summary of the resource, limited to 4,000 characters.&lt;/p&gt;&lt;p&gt;Example:&lt;/p&gt;&lt;p&gt;A mission and overview of the Data Inventory Program (DIP) containing instructions, references, terminology, and explanations designed  for users to understand and be able to use the features it contains.&lt;/p&gt;
+A summary of the resource, limited to 4,000 characters.
+Example:
+A mission and overview of the Data Inventory Program (DIP) containing instructions, references, terminology, and explanations designed  for users to understand and be able to use the features it contains.
 &lt;dcterms:description&gt;</t>
       </text>
     </comment>
     <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <t>keyword:
-&lt;p&gt;A keyword or multiple (comma delimited) keywords describing the resource.&lt;/p&gt;&lt;p&gt;Example:&lt;/p&gt;&lt;p&gt;City of New York, Universities, Immigration&lt;/p&gt;
+A keyword or multiple (comma delimited) keywords describing the resource.
+Example:
+City of New York, Universities, Immigration
 &lt;dcat:keyword&gt;</t>
       </text>
     </comment>
     <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <t>publisher:
-&lt;p&gt;The entity responsible for making the resource available.&lt;/p&gt;&lt;p&gt;Entity may include federal agency, sub- agency, state or local agencies, an organization, a network, a service, or a POC.&lt;/P&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;DHS/MGMT/OCHCO&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The entity responsible for making the resource available.
+Entity may include federal agency, sub- agency, state or local agencies, an organization, a network, a service, or a POC.
+Example:
+DHS/MGMT/OCHCO
 &lt;dcterms:publisher&gt;</t>
       </text>
     </comment>
     <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <t>accessLevel:
-&lt;p&gt;The three levels that determine how publicly-available the resource is:&lt;/p&gt;&lt;p&gt;Public: is/could be publicly-available without restrictions.&lt;/p&gt;&lt;p&gt;Restricted Public: is available under certain restrictions.&lt;/p&gt;&lt;p&gt;Non-Public: is not available to the public.&lt;/p&gt;
+The three levels that determine how publicly-available the resource is:
+Public: is/could be publicly-available without restrictions.
+Restricted Public: is available under certain restrictions.
+Non-Public: is not available to the public.
 &lt;usg:accessLevel&gt;</t>
       </text>
     </comment>
     <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <t>dataCatalogRecordAccessLevel:
-&lt;p&gt;The classification of this Data Inventory Record as either Public or Non-Public.&lt;/p&gt;&lt;p&gt;Can this record be published in data.gov?&lt;ul class='no-bullets'&gt;&lt;li&gt;Yes = Public&lt;/li&gt;&lt;li&gt;No = Non-Public&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The classification of this Data Inventory Record as either Public or Non-Public.
+Can this record be published in data.gov?
+Yes = Public
+No = Non-Public
 &lt;dhs:dataCatalogRecordAccessLevel&gt;</t>
       </text>
     </comment>
     <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <t>issued:
-&lt;p&gt;The issued date of the dataset (if not published this may be the date the data was first made available internally).&lt;/p&gt;&lt;p&gt;Records submitted via JSON must be in ISO 8601 format (YYYY-MM-DD). Records submitted via Excel must be in standard format (MM/DD/YYYY).&lt;/p&gt;
+The issued date of the dataset (if not published this may be the date the data was first made available internally).
+Records submitted via JSON must be in ISO 8601 format (YYYY-MM-DD). Records submitted via Excel must be in standard format (MM/DD/YYYY).
 &lt;dcterms:issued&gt;</t>
       </text>
     </comment>
     <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <t>component:
-&lt;p&gt;The DHS Component (sub-agency) the data pertains too.&lt;/p&gt;&lt;p&gt;&lt;ul class='no-bullets'&gt;&lt;li&gt;MGMT&lt;/li&gt;&lt;li&gt;CISA&lt;/li&gt;&lt;li&gt;CBP&lt;/li&gt;&lt;li&gt;&lt;/li&gt;&lt;li&gt;FEMA&lt;/li&gt;&lt;li&gt;S&amp;T&lt;/li&gt;&lt;li&gt;TSA&lt;/li&gt;&lt;li&gt;ICE&lt;/li&gt;&lt;li&gt;USCIS&lt;/li&gt;&lt;li&gt;FPS&lt;/li&gt;&lt;li&gt;FLETC&lt;/li&gt;&lt;li&gt;USSS&lt;/li&gt;&lt;li&gt;USCG&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The DHS Component (sub-agency) the data pertains too.
+MGMT
+CISA
+CBP
+FEMA
+S&amp;T
+TSA
+ICE
+USCIS
+FPS
+FLETC
+USSS
+USCG
 &lt;dhs:component&gt;</t>
       </text>
     </comment>
     <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <t>restrictionReason:
-&lt;p&gt;A reason for which the dataset is not published to data.gov (I.e. not marked as 'public' for accessLevel and not marked as 'public' for dataCatalogRecordAccessLevel). Must be provided as a comma separated list including one or more of the following:&lt;/p&gt;&lt;p&gt;&lt;ul class='no-bullets'&gt;&lt;li&gt;PII Sensitive&lt;/li&gt;&lt;li&gt;Security Risk&lt;/li&gt;&lt;li&gt;Legal liability&lt;/li&gt;&lt;li&gt;Intellectual Property Rights&lt;/li&gt;&lt;li&gt;Confidential Business Information&lt;/li&gt;&lt;li&gt;Restricted by Contract&lt;/li&gt;&lt;li&gt;FOIA Exeption&lt;/li&gt;&lt;li&gt;OMB Director Discretion&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+A reason for which the dataset is not published to data.gov (I.e. not marked as 'public' for accessLevel and not marked as 'public' for dataCatalogRecordAccessLevel). Must be provided as a comma separated list including one or more of the following:
+PII Sensitive
+Security Risk
+Legal Liability
+Intellectual Property Rights
+Confidential Business Information
+Restricted by Contract
+FOIA Exemption
+OMB Director Discretion
 &lt;dhs:restrictionReason&gt;</t>
       </text>
     </comment>
     <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <t>creator:
-&lt;p&gt;Either a name or email (individual or group) of the individual responsible for creating the resource. Include the point of contact information with either a name or email (individual or group) when submitting via Excel or a full Vcard when submitting via JSON.&lt;/p&gt;
+Either a name or email (individual or group) of the individual responsible for creating the resource. Include the point of contact information with either a name or email (individual or group) when submitting via Excel or a full Vcard when submitting via JSON.
 &lt;dcterms:creator&gt;</t>
       </text>
     </comment>
     <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <t>governance:
-&lt;p&gt;Either a name or email (individual or group) of the individual responsible for overseeing the information contained in the resource. Include the point of contact information with  either a name or email (individual or group) when submitting via Excel or a full Vcard when submitting via JSON.&lt;/p&gt;
+Either a name or email (individual or group) of the individual responsible for overseeing the information contained in the resource. Include the point of contact information with  either a name or email (individual or group) when submitting via Excel or a full Vcard when submitting via JSON.
 &lt;dhs:governance&gt;</t>
       </text>
     </comment>
     <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <t>owner:
-&lt;p&gt;Either a name or email (individual or group) of the individual responsible for the accuracy of the information contained in the resource when submitting via Excel or a full Vcard when submitting via JSON.&lt;/p&gt;
+Either a name or email (individual or group) of the individual responsible for the accuracy of the information contained in the resource when submitting via Excel or a full Vcard when submitting via JSON.
 &lt;dhs:owner&gt;</t>
       </text>
     </comment>
     <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <t>steward:
-&lt;p&gt;Either a name or email (individual or group) of the administrator of the dataset who ensures the information is properly stored, maintained, accessible, and protected. If submitting via JSON, a full Vcard.&lt;/p&gt;
+Either a name or email (individual or group) of the administrator of the dataset who ensures the information is properly stored, maintained, accessible, and protected. If submitting via JSON, a full Vcard.
 &lt;dhs:steward&gt;</t>
       </text>
     </comment>
     <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <t>custodian:
-&lt;p&gt;Either a name or email (individual or group) of the individual who has physical possession of the information. If submitting via JSON, a full Vcard.&lt;/p&gt;
+Either a name or email (individual or group) of the individual who has physical possession of the information. If submitting via JSON, a full Vcard.
 &lt;dhs:custodian&gt;</t>
       </text>
     </comment>
     <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <t>primaryITInvestmentUII:
-&lt;p&gt;Used for linking a dataset with an IT UII. A Unique Investment Identifier (UII) is an established and unique identifier of an investment, assigned at the Component level.&lt;/p&gt;&lt;p&gt;Example: 010-999992220&lt;/p&gt;&lt;p&gt;Non-Tech Example: The number/ identifier on the 'Property of...' sticker on your laptop.&lt;/p&gt;
+Used for linking a dataset with an IT UII. A Unique Investment Identifier (UII) is an established and unique identifier of an investment, assigned at the Component level.
+Example: 010-999992220
+Non-Tech Example: The number/ identifier on the 'Property of...' sticker on your laptop.
 &lt;usg:primaryITInvestmentUII&gt;</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <t>fismaID:
-&lt;p&gt;The FISMA ID is a unique identifier that describes various key characteristics of a specific system.&lt;/p&gt;&lt;p&gt;If the dataset is part of a system that has a FISMA ID then the FISMA ID should be provided.&lt;/p&gt;&lt;p&gt;Example:&lt;/p&gt;&lt;ul class='no-bullets'&gt;&lt;li&gt;FSA-00100-MAJ-00100&lt;/li&gt;&lt;li&gt;- OR -&lt;/li&gt;&lt;li&gt;TSA-02379-SUB-00465&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The FISMA ID is a unique identifier that describes various key characteristics of a specific system.
+If the dataset is part of a system that has a FISMA ID then the FISMA ID should be provided.
+Example:
+FSA-00100-MAJ-00100
+- OR -
+TSA-02379-SUB-00465
 &lt;dhs:fismaID&gt;</t>
       </text>
     </comment>
     <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <t>references:
-&lt;p&gt;A related piece of information from another source (typically linked via URL) that provides additional related information about the resource.&lt;/p&gt;
+A related piece of information from another source (typically linked via URL) that provides additional related information about the resource.
 &lt;dcterms:references&gt;</t>
       </text>
     </comment>
     <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <t>sharingAgreements:
-&lt;p&gt;A contract that states what and how  information can be shared or utilized.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://www.dhs.gov/sites/default/files/publications/privacy_crcl_guidance_ise_2009-01_0.pdf&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;&lt;p&gt;DHS&lt;/p&gt;&lt;p&gt;&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/fingerprint&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+A contract that states what and how  information can be shared or utilized.
+Example:
+https://www.dhs.gov/sites/default/files/publications/privacy_crcl_guidance_ise_2009-01_0.pdf
+DHS
+https://catalog.data.gov/dataset/fingerprint
 &lt;dhs:sharingAgreements&gt;</t>
       </text>
     </comment>
     <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <t>contactPoint:
-&lt;p&gt;The contact information  (name and email preferred) of the main individual to contact with questions about the dataset.&lt;/p&gt;
+The contact information  (name and email preferred) of the main individual to contact with questions about the dataset.
 &lt;dcat:contactPoint&gt;</t>
       </text>
     </comment>
     <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <t>collectionAuthority:
-&lt;p&gt;The legislation or executive order under which the data was collected.&lt;/p&gt;&lt;p&gt;The specific document or policy that grants you permission to collect specific data.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://www.ecfr.gov/current/title-28/chapter-I/part-28/subpart-B/section-28.12&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The legislation or executive order under which the data was collected.
+The specific document or policy that grants you permission to collect specific data.
+Example:
+https://www.ecfr.gov/current/title-28/chapter-I/part-28/subpart-B/section-28.12
 &lt;dhs:collectionAuthority&gt;</t>
       </text>
     </comment>
     <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <t>releaseAuthority:
-&lt;p&gt;The document, legislation or executive order under which he data can be released.&lt;/p&gt;&lt;p&gt;Examples:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://www.ecfr.gov/current/title-6/chapter-I/part-7/subpart-B/section-7.23&lt;/li&gt;&lt;li&gt;https://irp.fas.org/dni/icd/icd-403.pdf&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;
+The document, legislation or executive order under which he data can be released.
+Examples:
+https://www.ecfr.gov/current/title-6/chapter-I/part-7/subpart-B/section-7.23
+https://irp.fas.org/dni/icd/icd-403.pdf
 &lt;dhs:releaseAuthority&gt;</t>
       </text>
     </comment>
     <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <t>recordsSchedule:
-&lt;p&gt;The policy indicating the time period in which the records are retained.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;DAA-0563-2013-0005 (link below)&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The policy indicating the time period in which the records are retained.
+Example:
+DAA-0563-2013-0005 (link below)
 &lt;dhs:recordsSchedule&gt;</t>
       </text>
     </comment>
     <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <t>systemOfRecords:
-&lt;p&gt;If the system is designated as a system of records under the Privacy Act of 1974, provide the URL to the System of Records Notice that relates to the dataset. The URL should be from FederalRegister.gov  or point to an entry from the Federal Register.&lt;/p&gt;
+If the system is designated as a system of records under the Privacy Act of 1974, provide the URL to the System of Records Notice that relates to the dataset. The URL should be from FederalRegister.gov  or point to an entry from the Federal Register.
 &lt;usg:systemOfRecords&gt;</t>
       </text>
     </comment>
     <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <t>ptaAdjudicatedDate:
-&lt;p&gt;The date on which the Privacy Threshold Assessment (PTA) was adjudicated&lt;/p&gt;
+The date on which the Privacy Threshold Assessment (PTA) was adjudicated
 &lt;dhs:ptaAdjudicatedDate&gt;</t>
       </text>
     </comment>
     <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <t>conformsTo:
-&lt;p&gt;A technical standard that the dataset conforms to.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;WGS84 is standard for GPS. The Global Positioning System uses the World Geodetic System (WGS84) as its reference coordinate system.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+A technical standard that the dataset conforms to.
+Example:
+WGS84 is standard for GPS. The Global Positioning System uses the World Geodetic System (WGS84) as its reference coordinate system.
 &lt;dcterms:conformsTo&gt;</t>
       </text>
     </comment>
     <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <t>conformsFIPS:
-&lt;p&gt;The Federal Inventory Processing Standard that the dataset conforms to, if any.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;FIPS201-3&lt;/li&gt;&lt;li&gt;https://csrc.nist.gov/publications/detail/fips/201/3/final&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The Federal Inventory Processing Standard that the dataset conforms to, if any.
+Example:
+FIPS201-3
+https://csrc.nist.gov/publications/detail/fips/201/3/final
 &lt;dhs:conformsFIPS&gt;</t>
       </text>
     </comment>
     <comment ref="AB1" authorId="0" shapeId="0">
       <text>
         <t>conformsNIEMPercent:
-&lt;p&gt;The numerical percentage (0-100) of the dataset that is NIEM compliant.&lt;/p&gt;
+The numerical percentage (0-100) of the dataset that is NIEM compliant.
 &lt;dhs:conformsNIEMPercent&gt;</t>
       </text>
     </comment>
     <comment ref="AC1" authorId="0" shapeId="0">
       <text>
         <t>conformsUnicode:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Is the information in the resource written in Unicode (does the code given to each character start with the letter 'u')?&lt;/p&gt;&lt;p&gt;Information containing foreign languages/characters are typically written in Unicode format (U+XXX).&lt;/p&gt;
+True or False
+Is the information in the resource written in Unicode (does the code given to each character start with the letter 'u')?
+Information containing foreign languages/characters are typically written in Unicode format (U+XXX).
 &lt;dhs:conformsUnicode&gt;</t>
       </text>
     </comment>
     <comment ref="AD1" authorId="0" shapeId="0">
       <text>
         <t>identitiesNativeScript:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Are the names of individuals and other entities stored in a way (e.g. Roman characters) that can be shared across systems?&lt;/p&gt;
+True or False
+Are the names of individuals and other entities stored in a way (e.g. Roman characters) that can be shared across systems?
 &lt;dhs:identitiesNativeScript&gt;</t>
       </text>
     </comment>
     <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <t>transliterationStandard:
-&lt;p&gt;The standard of converting  text  from one language to Roman characters.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://www.iso.org/ics/01.140.10/x/&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The standard of converting  text  from one language to Roman characters.
+Example:
+https://www.iso.org/ics/01.140.10/x/
 &lt;dhs:transliterationStandard&gt;</t>
       </text>
     </comment>
     <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <t>sourceDatasets:
-&lt;p&gt;An identifier for the originating dataset (the DHS Unique Identifier if possible or DOI or URL for externally developed datasets).&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;Mobius - creates TRM Data which TRM team uses for various projects.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+An identifier for the originating dataset (the DHS Unique Identifier if possible or DOI or URL for externally developed datasets).
+Example:
+Mobius - creates TRM Data which TRM team uses for various projects.
 &lt;dhs:sourceDatasets&gt;</t>
       </text>
     </comment>
     <comment ref="AG1" authorId="0" shapeId="0">
       <text>
         <t>destinationDatasets:
-&lt;p&gt;The unique identifier of downstream datasets fed by this dataset.&lt;/p&gt;&lt;P&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;In this instance, Mobius would include the unique identifier for downstream datasets.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The unique identifier of downstream datasets fed by this dataset.
+&lt;P&gt;Example:
+In this instance, Mobius would include the unique identifier for downstream datasets.
 &lt;dhs:destinationDatasets&gt;</t>
       </text>
     </comment>
     <comment ref="AH1" authorId="0" shapeId="0">
       <text>
         <t>describedBy:
-&lt;p&gt;A URL link to the  dictionary that defines the fields or column heading of the information.&lt;/p&gt;
+A URL link to the  dictionary that defines the fields or column heading of the information.
 &lt;usg:describedBy&gt;</t>
       </text>
     </comment>
     <comment ref="AI1" authorId="0" shapeId="0">
       <text>
         <t>describedByType:
-&lt;p&gt;The file format of the describedBy URL link. Should be a standard mime (IANA media)type.&lt;/p&gt;&lt;p&gt;Examples:&lt;ul class='no-bullets'&gt;&lt;li&gt;application/xml&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The file format of the describedBy URL link. Should be a standard mime (IANA media)type.
+Examples:
+application/xml
 &lt;usg:describedByType&gt;</t>
       </text>
     </comment>
     <comment ref="AJ1" authorId="0" shapeId="0">
       <text>
         <t>isPartOf:
-&lt;p&gt;The source in which a grouping of related resources are included in. This is typically the name of the system in which the dataset resides.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;TRM isPartOf Mobius.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The source in which a grouping of related resources are included in. This is typically the name of the system in which the dataset resides.
+Example:
+TRM isPartOf Mobius.
 &lt;dcterms:isPartOf&gt;</t>
       </text>
     </comment>
     <comment ref="AK1" authorId="0" shapeId="0">
       <text>
         <t>isOpenSource:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The data in the dataset is composed of publicly available data and maybe compiled from multiple sources.&lt;/p&gt;
+True or False
+The data in the dataset is composed of publicly available data and maybe compiled from multiple sources.
 &lt;dhs:isOpenSource&gt;</t>
       </text>
     </comment>
     <comment ref="AL1" authorId="0" shapeId="0">
       <text>
         <t>isCommercial:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The dataset is aquired from a private sector provider (may be purchased or acquired via agreement).&lt;/p&gt;
+True or False
+The dataset is aquired from a private sector provider (may be purchased or acquired via agreement).
 &lt;dhs:isCommercial&gt;</t>
       </text>
     </comment>
     <comment ref="AM1" authorId="0" shapeId="0">
       <text>
         <t>hasDataDictionary:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The dataset has a data dictionary (should be pointed to in the referencedBy attribute).&lt;/p&gt;
+True or False
+The dataset has a data dictionary (should be pointed to in the referencedBy attribute).
 &lt;dhs:hasDataDictionary&gt;</t>
       </text>
     </comment>
     <comment ref="AN1" authorId="0" shapeId="0">
       <text>
         <t>accrualPeriodicity:
-&lt;p&gt;The frequency with which resources or sets of information are added to the dataset. Recommend timeframes (or frequency) can be found in the Collection Description Accrual Policy Vocabulary. &lt;/p&gt;
+The frequency with which resources or sets of information are added to the dataset. Recommend timeframes (or frequency) can be found in the Collection Description Accrual Policy Vocabulary. 
 &lt;dcterms:accrualPeriodicity&gt;</t>
       </text>
     </comment>
     <comment ref="AO1" authorId="0" shapeId="0">
       <text>
         <t>spatial:
-&lt;p&gt;A named local or geographic area.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;St. Elizabeth Campus, Downtown DC, Arlington County, United States&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+A named local or geographic area.
+Example:
+St. Elizabeth Campus, Downtown DC, Arlington County, United States
 &lt;dcterms:spatial&gt;</t>
       </text>
     </comment>
     <comment ref="AP1" authorId="0" shapeId="0">
       <text>
         <t>spatialResolutionInMeters:
-&lt;p&gt;How small of an area, in meters, you can make (or zoom into) an image that will still provide a quality resolution in order to identify the content in the image.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;5x5 meters&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+How small of an area, in meters, you can make (or zoom into) an image that will still provide a quality resolution in order to identify the content in the image.
+Example:
+5x5 meters
 &lt;dcat:spatialResolutionInMeters&gt;</t>
       </text>
     </comment>
     <comment ref="AQ1" authorId="0" shapeId="0">
       <text>
         <t>temporal:
-&lt;p&gt;The period of time that the dataset covers.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;December 2021&lt;/li&gt;&lt;li&gt;2012-2018&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The period of time that the dataset covers.
+Example:
+December 2021
+2012-2018
 &lt;dcterms:temporal&gt;</t>
       </text>
     </comment>
     <comment ref="AR1" authorId="0" shapeId="0">
       <text>
         <t>temporalResolution:
-&lt;p&gt;The smallest amount of time between records in dataset.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;P1Y&lt;/li&gt;&lt;li&gt;P1M&lt;/li&gt;&lt;li&gt;P7D&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The smallest amount of time between records in dataset.
+Example:
+P1Y
+P1M
+P7D
 &lt;dcat:temporalResolution&gt;</t>
       </text>
     </comment>
     <comment ref="AS1" authorId="0" shapeId="0">
       <text>
         <t>dataQualityKnown:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Is the quality of the information in the resource known?&lt;/p&gt;
+True or False
+Is the quality of the information in the resource known?
 &lt;dhs:dataQualityKnown&gt;</t>
       </text>
     </comment>
     <comment ref="AT1" authorId="0" shapeId="0">
       <text>
         <t>dataQualityPercent:
-&lt;p&gt;A simple measure of the data quality, on a scale of 0-100.&lt;/p&gt;
+A simple measure of the data quality, on a scale of 0-100.
 &lt;dhs:dataQualityPercent&gt;</t>
       </text>
     </comment>
     <comment ref="AU1" authorId="0" shapeId="0">
       <text>
         <t>dataQualityAssessment:
-&lt;p&gt;A written account evaluating the quality of the information contained within the resource.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;This dataset has some gaps in critical areas. Efforts are underway to remediate.&lt;/li&gt;&lt;li&gt;&amp;nbsp;&lt;/li&gt;&lt;li&gt;This dataset is based on information obtained in 2017. Efforts underway to obtain current data.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+A written account evaluating the quality of the information contained within the resource.
+Example:
+This dataset has some gaps in critical areas. Efforts are underway to remediate.
+&amp;nbsp;
+This dataset is based on information obtained in 2017. Efforts underway to obtain current data.
 &lt;dhs:dataQualityAssessment&gt;</t>
       </text>
     </comment>
     <comment ref="AV1" authorId="0" shapeId="0">
       <text>
         <t>dataQuality:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Does the information contained in the resource meet the agency's Information Quality Guidelines?&lt;/p&gt;
+True or False
+Does the information contained in the resource meet the agency's Information Quality Guidelines?
 &lt;usg:dataQuality&gt;</t>
       </text>
     </comment>
     <comment ref="AW1" authorId="0" shapeId="0">
       <text>
         <t>format:
-&lt;p&gt;The file format, physical medium, or dimension of the resource.&lt;/p&gt;&lt;p&gt;Examples:&lt;ul class='no-bullets'&gt;&lt;li&gt;File Format - CSV, HTML, JSON, MySQL&lt;/li&gt;&lt;li&gt;Physical Medium - USB drives, CD&lt;li&gt;&lt;li&gt;Dimension - Size, Duration&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The file format, physical medium, or dimension of the resource.
+Examples:
+File Format - CSV, HTML, JSON, MySQL
+Physical Medium - USB drives, CD
+Dimension - Size, Duration
 &lt;dcterms:format&gt;</t>
       </text>
     </comment>
     <comment ref="AX1" authorId="0" shapeId="0">
       <text>
         <t>accessURL:
-&lt;p&gt;The landing page (URL) that gives access to the resource.&lt;/p&gt;&lt;p&gt;Must be a URL.&lt;/p&gt;&lt;p&gt;https://ea.dhs.gov/mobius&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;The Netflix login page your required to complete in order to gain access to their content.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The landing page (URL) that gives access to the resource.
+Must be a URL.
+https://ea.dhs.gov/mobius
+Example:
+The Netflix login page your required to complete in order to gain access to their content.
 &lt;dcat:accessURL&gt;</t>
       </text>
     </comment>
     <comment ref="AY1" authorId="0" shapeId="0">
       <text>
         <t>accessURLNIEM:
-&lt;p&gt;The landing page (URL) that provides you access to the NIEM interface.&lt;/p&gt;&lt;p&gt;Must be a URL.&lt;/p&gt;
+The landing page (URL) that provides you access to the NIEM interface.
+Must be a URL.
 &lt;dhs:accessURLNIEM&gt;</t>
       </text>
     </comment>
     <comment ref="AZ1" authorId="0" shapeId="0">
       <text>
         <t>modified:
-&lt;p&gt;The most recent date on  which the information contained in the resource was changed, updated, or modified.&lt;p&gt;
+The most recent date on  which the information contained in the resource was changed, updated, or modified.
 &lt;usg:modified&gt;</t>
       </text>
     </comment>
     <comment ref="BA1" authorId="0" shapeId="0">
       <text>
         <t>vendor:
-The vendor, supplier, or set of suppliers who supplied the information contained in the resource.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;ECS&lt;/li&gt;&lt;li&gt;ECS, GeoMgmt Inc.&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The vendor, supplier, or set of suppliers who supplied the information contained in the resource.
+Example:
+ECS
+ECS, GeoMgmt Inc.
 &lt;dhs:vendor&gt;</t>
       </text>
     </comment>
     <comment ref="BB1" authorId="0" shapeId="0">
       <text>
         <t>license:
-&lt;p&gt;The legal structure that gives official permission to utilize or  distribute information contained in the resource.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;MIT&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The legal structure that gives official permission to utilize or  distribute information contained in the resource.
+Example:
+MIT
 &lt;dcterms:license&gt;</t>
       </text>
     </comment>
     <comment ref="BC1" authorId="0" shapeId="0">
       <text>
         <t>accessRights:
-&lt;p&gt;Provides information regarding access or restrictions to data based on privacy, security, or other policies&lt;/p&gt;&lt;p&gt;Example:&lt;/p&gt;&lt;p&gt;User must have PIV card and be granted permission by System Owner&lt;/p&gt;
+Provides information regarding access or restrictions to data based on privacy, security, or other policies
+Example:
+User must have PIV card and be granted permission by System Owner
 &lt;dcterms:accessRights&gt;</t>
       </text>
     </comment>
     <comment ref="BD1" authorId="0" shapeId="0">
       <text>
         <t>theme:
-&lt;p&gt;The main category of the information contained in the resource. A resource can have multiple themes.&lt;/p&gt;&lt;p&gt;Theme is similar to a Keyword but at a much higher level.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;Policy&lt;/li&gt;&lt;li&gt;Data Mgmt.&lt;/li&gt;&lt;li&gt;Data Inventory&lt;/li&gt;&lt;li&gt;Data Governance&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The main category of the information contained in the resource. A resource can have multiple themes.
+Theme is similar to a Keyword but at a much higher level.
+Example:
+Policy
+Data Mgmt.
+Data Inventory
+Data Governance
 &lt;dcat:theme&gt;</t>
       </text>
     </comment>
     <comment ref="BE1" authorId="0" shapeId="0">
       <text>
         <t>functionalDataDomain:
-&lt;p&gt;The functional subject area of the resource.&lt;/p&gt;&lt;p&gt;List:&lt;ul class='no-bullets'&gt;&lt;li&gt;Biometrics&lt;/li&gt;&lt;li&gt;CBRN&lt;/li&gt;&lt;li&gt;Cybersecurity&lt;/li&gt;&lt;li&gt;Emergency Mgmt. Geospatial&lt;/li&gt;&lt;li&gt;Immigration&lt;/li&gt;&lt;li&gt;Infra. Protection&lt;/li&gt;&lt;li&gt;Intelligence&lt;/li&gt;&lt;li&gt;International Trade&lt;/li&gt;&lt;li&gt;Law Enforcement&lt;/li&gt;&lt;li&gt;Maritime&lt;/li&gt;&lt;li&gt;Mission Support &amp; Mgmt.&lt;/li&gt;&lt;li&gt;Screening&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The functional subject area of the resource.
+List:
+Biometrics
+CBRN
+Cybersecurity
+Emergency Mgmt. Geospatial
+Immigration
+Infra. Protection
+Intelligence
+International Trade
+Law Enforcement
+Maritime
+Mission Support &amp; Mgmt.
+Screening
 &lt;dhs:functionalDataDomain&gt;</t>
       </text>
     </comment>
     <comment ref="BF1" authorId="0" shapeId="0">
       <text>
         <t>mediaType:
-&lt;p&gt;The media type of the distribution as defined by IANA.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;application/node&lt;/li&gt;&lt;li&gt;audio/mp4&lt;/li&gt;&lt;li&gt;font/otf&lt;/li&gt;&lt;li&gt;image/png&lt;/li&gt;&lt;li&gt;message/http&lt;/li&gt;&lt;li&gt;model/obj&lt;/li&gt;&lt;li&gt;text/csv&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The media type of the distribution as defined by IANA.
+Example:
+application/node
+audio/mp4
+font/otf
+image/png
+message/http
+model/obj
+text/csv
 &lt;dcat:mediaType&gt;</t>
       </text>
     </comment>
     <comment ref="BG1" authorId="0" shapeId="0">
       <text>
         <t>isStream:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Data Set or Data Source is streaming. The data is constantly updated.&lt;/p&gt;
+True or False
+Data Set or Data Source is streaming. The data is constantly updated.
 &lt;dhs:isStream&gt;</t>
       </text>
     </comment>
     <comment ref="BH1" authorId="0" shapeId="0">
       <text>
         <t>accessInstructions:
-&lt;p&gt;The steps or actions an individual must take to gain access to the dataset. Can work in conjunction with accessRights (max length 5,000 characters).&lt;/p&gt;&lt;p&gt;Example: 'Visit the (accessURL) link and then click on 'Your ArcGIS organization's URL and enter &lt;MGMT&gt; and click Continue'&lt;/p&gt;
+The steps or actions an individual must take to gain access to the dataset. Can work in conjunction with accessRights (max length 5,000 characters).
+Example: 'Visit the (accessURL) link and then click on 'Your ArcGIS organization's URL and enter &lt;MGMT&gt; and click Continue'
 &lt;dhs:accessInstructions&gt;</t>
       </text>
     </comment>
     <comment ref="BI1" authorId="0" shapeId="0">
       <text>
         <t>tableCount:
-&lt;p&gt;The number of 2-dimensional tables in the data.&lt;/p&gt;
+The number of 2-dimensional tables in the data.
 &lt;dhs:tableCount&gt;</t>
       </text>
     </comment>
     <comment ref="BJ1" authorId="0" shapeId="0">
       <text>
         <t>recordCount:
-&lt;p&gt;The total number of records in the data.&lt;/p&gt;
+The total number of records in the data.
 &lt;dhs:recordCount&gt;</t>
       </text>
     </comment>
     <comment ref="BK1" authorId="0" shapeId="0">
       <text>
         <t>byteSize:
-&lt;p&gt;The size of the distribution in bytes.&lt;/p&gt;&lt;p&gt;The size in bytes can be approximated (as a integer) when the precise size is not known.&lt;/p&gt;
+The size of the distribution in bytes.
+The size in bytes can be approximated (as a integer) when the precise size is not known.
 &lt;dcat:byteSize&gt;</t>
       </text>
     </comment>
     <comment ref="BL1" authorId="0" shapeId="0">
       <text>
         <t>datasetClassification:
-&lt;p&gt;The security classification of the data.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;CUI&lt;/li&gt;&lt;li&gt;Confidential&lt;/li&gt;&lt;li&gt;Secret&lt;/li&gt;&lt;li&gt;Top Secret&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The security classification of the data.
+Example:
+CUI
+Confidential
+Secret
+Top Secret
 &lt;dhs:datasetClassification&gt;</t>
       </text>
     </comment>
     <comment ref="BM1" authorId="0" shapeId="0">
       <text>
         <t>ch-person-level:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains enough personal records or enough personal information in order to identify an individual.&lt;/p&gt;
+True or False
+The information in the resource contains enough personal records or enough personal information in order to identify an individual.
 &lt;dhs:ch-person-level&gt;</t>
       </text>
     </comment>
     <comment ref="BN1" authorId="0" shapeId="0">
       <text>
         <t>ch-financial:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains financial information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;Bank Statements&lt;/li&gt;&lt;li&gt;Credit Reports&lt;/li&gt;&lt;li&gt;W2&lt;/li&gt;&lt;li&gt;Net Worth&lt;/li&gt;&lt;li&gt;Bank Secrecy&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains financial information.
+Example:
+Bank Statements
+Credit Reports
+W2
+Net Worth
+Bank Secrecy
 &lt;dhs:ch-financial&gt;</t>
       </text>
     </comment>
     <comment ref="BO1" authorId="0" shapeId="0">
       <text>
         <t>ch-event-records:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains information about events which are tagged with a specific place and time.&lt;/p&gt;
+True or False
+The information in the resource contains information about events which are tagged with a specific place and time.
 &lt;dhs:ch-event-records&gt;</t>
       </text>
     </comment>
     <comment ref="BP1" authorId="0" shapeId="0">
       <text>
         <t>ch-faces:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains facial recognition data or images of human faces.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/global-entry-master-dataset&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains facial recognition data or images of human faces.
+Example:
+https://catalog.data.gov/dataset/global-entry-master-dataset
 &lt;dhs:ch-faces&gt;</t>
       </text>
     </comment>
     <comment ref="BQ1" authorId="0" shapeId="0">
       <text>
         <t>ch-fingerprints:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains fingerprint data or images of fingerprints.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/global-entry-master-dataset&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains fingerprint data or images of fingerprints.
+Example:
+https://catalog.data.gov/dataset/global-entry-master-dataset
 &lt;dhs:ch-fingerprints&gt;</t>
       </text>
     </comment>
     <comment ref="BR1" authorId="0" shapeId="0">
       <text>
         <t>ch-cui:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains Controlled Unclassified Information (CUI).&lt;/p&gt;
+True or False
+The information in the resource contains Controlled Unclassified Information (CUI).
 &lt;dhs:ch-cui&gt;</t>
       </text>
     </comment>
     <comment ref="BS1" authorId="0" shapeId="0">
       <text>
         <t>ch-phi:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains Protected Health Information (PHI).&lt;/p&gt;&lt;p&gt;Examples:&lt;ul class='no-bullets'&gt;&lt;li&gt;Medical Records&lt;/li&gt;&lt;li&gt;Diagnoses&lt;/li&gt;&lt;li&gt;Medicul Results&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains Protected Health Information (PHI).
+Examples:
+Medical Records
+Diagnoses
+Medicul Results
 &lt;dhs:ch-phi&gt;</t>
       </text>
     </comment>
     <comment ref="BT1" authorId="0" shapeId="0">
       <text>
         <t>ch-pii:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains Personally Identifiable Information (PII).&lt;/p&gt;&lt;p&gt;Reference: &lt;a href='https://www.dhs.gov/sites/default/files/publications/dhs%20policy%20directive%20047-01-007%20handbook%20for%20safeguarding%20sensitive%20PII%2012-4-2017.pdf'&gt;https://www.dhs.gov/sites/default/files/publications/dhs%20policy%20directive%20047-01-007%20handbook%20for%20safeguarding%20sensitive%20PII%2012-4-2017.pdf&lt;/a&gt;&lt;/p&gt;
+True or False
+The information in the resource contains Personally Identifiable Information (PII).
+Reference: &lt;a href='https://www.dhs.gov/sites/default/files/publications/dhs%20policy%20directive%20047-01-007%20handbook%20for%20safeguarding%20sensitive%20PII%2012-4-2017.pdf'&gt;https://www.dhs.gov/sites/default/files/publications/dhs%20policy%20directive%20047-01-007%20handbook%20for%20safeguarding%20sensitive%20PII%2012-4-2017.pdf&lt;/a&gt;
 &lt;dhs:ch-pii&gt;</t>
       </text>
     </comment>
     <comment ref="BU1" authorId="0" shapeId="0">
       <text>
         <t>ch-geospatial:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains geospatial information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/fema-historical-disaster-declarations-shp&lt;/li&gt;&lt;li&gt;https://catalog.data.gov/dataset/formerly-used-defense-sites-fuds-public-properties&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains geospatial information.
+Example:
+https://catalog.data.gov/dataset/fema-historical-disaster-declarations-shp
+https://catalog.data.gov/dataset/formerly-used-defense-sites-fuds-public-properties
 &lt;dhs:ch-geospatial&gt;</t>
       </text>
     </comment>
     <comment ref="BV1" authorId="0" shapeId="0">
       <text>
         <t>ch-environmental:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains environmental information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/environmental-planning-historic-preservation-2dedc&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains environmental information.
+Example:
+https://catalog.data.gov/dataset/environmental-planning-historic-preservation-2dedc
 &lt;dhs:ch-environmental&gt;</t>
       </text>
     </comment>
     <comment ref="BW1" authorId="0" shapeId="0">
       <text>
         <t>ch-fisa:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains information pertaining to the Foreign Intelligence Surveillance Act (FISA).&lt;/p&gt;
+True or False
+The information in the resource contains information pertaining to the Foreign Intelligence Surveillance Act (FISA).
 &lt;dhs:ch-fisa&gt;</t>
       </text>
     </comment>
     <comment ref="BX1" authorId="0" shapeId="0">
       <text>
         <t>ch-8usc1367:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains  8 USC 1367.&lt;/p&gt;&lt;p&gt;Reference: https://www.dhs.gov/sites/default/files/publications/dhs_foia_instruction_section_1367_information.pdf&lt;/p&gt;
+True or False
+The information in the resource contains  8 USC 1367.
+Reference: https://www.dhs.gov/sites/default/files/publications/dhs_foia_instruction_section_1367_information.pdf
 &lt;dhs:ch-8usc1367&gt;</t>
       </text>
     </comment>
     <comment ref="BY1" authorId="0" shapeId="0">
       <text>
         <t>ch-propin:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains propriety commercial information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/automated-commercial-environment-international-trade-data-system-master-dataset&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains propriety commercial information.
+Example:
+https://catalog.data.gov/dataset/automated-commercial-environment-international-trade-data-system-master-dataset
 &lt;dhs:ch-propin&gt;</t>
       </text>
     </comment>
     <comment ref="BZ1" authorId="0" shapeId="0">
       <text>
         <t>ch-immigration:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains information pertaining to immigration.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;Asylee&lt;/li&gt;&lt;li&gt;Resident Status&lt;/li&gt;&lt;li&gt;Visas&lt;/li&gt;&lt;li&gt;Victims of Human Trafficking&lt;/li&gt;&lt;li&gt; https://catalog.data.gov/dataset/immigration-statistics-ef958&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains information pertaining to immigration.
+Example:
+Asylee
+Resident Status
+Visas
+Victims of Human Trafficking
+ https://catalog.data.gov/dataset/immigration-statistics-ef958
 &lt;dhs:ch-immigration&gt;</t>
       </text>
     </comment>
     <comment ref="CA1" authorId="0" shapeId="0">
       <text>
         <t>ch-criticalInfrastructure:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains critical infrastructure information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/emergency-medical-service-ems-stations&lt;/li&gt;&lt;li&gt;https://catalog.data.gov/dataset/ilss-data&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains critical infrastructure information.
+Example:
+https://catalog.data.gov/dataset/emergency-medical-service-ems-stations
+https://catalog.data.gov/dataset/ilss-data
 &lt;dhs:ch-criticalInfrastructure&gt;</t>
       </text>
     </comment>
     <comment ref="CB1" authorId="0" shapeId="0">
       <text>
         <t>ch-pcii:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains protected critical infrastructure information.&lt;/p&gt;
+True or False
+The information in the resource contains protected critical infrastructure information.
 &lt;dhs:ch-pcii&gt;</t>
       </text>
     </comment>
     <comment ref="CC1" authorId="0" shapeId="0">
       <text>
         <t>ch-biometrics:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains biometric information.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;https://catalog.data.gov/dataset/global-entry-master-dataset&lt;/li&gt;&lt;li&gt;https://catalog.data.gov/dataset/arrival-departure-information-system-b3b75&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+True or False
+The information in the resource contains biometric information.
+Example:
+https://catalog.data.gov/dataset/global-entry-master-dataset
+https://catalog.data.gov/dataset/arrival-departure-information-system-b3b75
 &lt;dhs:ch-biometrics&gt;</t>
       </text>
     </comment>
     <comment ref="CD1" authorId="0" shapeId="0">
       <text>
         <t>ch-disseminationRestrictions:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information  has dissemination restrictions.&lt;/p&gt;
+True or False
+The information  has dissemination restrictions.
 &lt;dhs:ch-disseminationRestrictions&gt;</t>
       </text>
     </comment>
     <comment ref="CE1" authorId="0" shapeId="0">
       <text>
         <t>ch-les:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information in the resource contains information that is deemed Law Enforcement Sensative.&lt;/p&gt;
+True or False
+The information in the resource contains information that is deemed Law Enforcement Sensative.
 &lt;dhs:ch-les&gt;</t>
       </text>
     </comment>
     <comment ref="CF1" authorId="0" shapeId="0">
       <text>
         <t>ch-synthetic:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The data is created manually or artificially apart from the data generated by real-world events. This may include data that is generated for the purposes of modeling and may be generated by a computer simulation. The data approximates real data, but does not necessarily reflect the real world. This includes synthetically derived data (e.g. data that is created programmatically from a set of source data, typically with some algorithm applied)&lt;/p&gt;
+True or False
+The data is created manually or artificially apart from the data generated by real-world events. This may include data that is generated for the purposes of modeling and may be generated by a computer simulation. The data approximates real data, but does not necessarily reflect the real world. This includes synthetically derived data (e.g. data that is created programmatically from a set of source data, typically with some algorithm applied)
 &lt;dhs:ch-synthetic&gt;</t>
       </text>
     </comment>
     <comment ref="CG1" authorId="0" shapeId="0">
       <text>
         <t>ch-anonymized:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The identifying information in the resource has been removed or changed so that the individual cannot be identified.&lt;/p&gt;
+True or False
+The identifying information in the resource has been removed or changed so that the individual cannot be identified.
 &lt;dhs:ch-anonymized&gt;</t>
       </text>
     </comment>
     <comment ref="CH1" authorId="0" shapeId="0">
       <text>
         <t>hostingLocation:
-&lt;p&gt;Where the data is located?&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;CIRRUS&lt;/li&gt;&lt;li&gt;AWS GovCloud&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+Where the data is located?
+Example:
+CIRRUS
+AWS GovCloud
 &lt;dhs:hostingLocation&gt;</t>
       </text>
     </comment>
     <comment ref="CI1" authorId="0" shapeId="0">
       <text>
         <t>hostedInCloud:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;Is the dataset stored in the cloud?&lt;/p&gt;
+True or False
+Is the dataset stored in the cloud?
 &lt;dhs:hostedInCloud&gt;</t>
       </text>
     </comment>
     <comment ref="CJ1" authorId="0" shapeId="0">
       <text>
         <t>easilyAccessibleByCreatingComponent:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information can be easily accessed by individuals within the DHS component that created it?&lt;/p&gt;
+True or False
+The information can be easily accessed by individuals within the DHS component that created it?
 &lt;dhs:easilyAccessibleByCreatingComponent&gt;</t>
       </text>
     </comment>
     <comment ref="CK1" authorId="0" shapeId="0">
       <text>
         <t>easilyAccessibleByAllComponents:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information can be easily accessed by individuals within all of DHS?&lt;/p&gt;
+True or False
+The information can be easily accessed by individuals within all of DHS?
 &lt;dhs:easilyAccessibleByAllComponents&gt;</t>
       </text>
     </comment>
     <comment ref="CL1" authorId="0" shapeId="0">
       <text>
         <t>easilyAccessibleByGeneralPublic:
-&lt;p&gt;True or False&lt;/p&gt;&lt;p&gt;The information can be easily accessed by the general public?&lt;/p&gt;
+True or False
+The information can be easily accessed by the general public?
 &lt;dhs:easilyAccessibleByGeneralPublic&gt;</t>
       </text>
     </comment>
     <comment ref="CM1" authorId="0" shapeId="0">
       <text>
         <t>encryptionAlgorithm:
-&lt;p&gt;The specific encryption algorithm used to protect data at rest.&lt;/p&gt;&lt;p&gt;Can have multiple comma separated values.&lt;/p&gt;&lt;p&gt;Example:&lt;li&gt;3DES&lt;/li&gt;&lt;li&gt;AES&lt;/li&gt;&lt;li&gt;RSA&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The specific encryption algorithm used to protect data at rest.
+Can have multiple comma separated values.
+Example:
+3DES
+AES
+RSA
 &lt;usg:encryptionAlgorithm&gt;</t>
       </text>
     </comment>
     <comment ref="CN1" authorId="0" shapeId="0">
       <text>
         <t>recordTransmission:
-&lt;p&gt;The date of when the information was submitted into the system.&lt;/p&gt;
+The date of when the information was submitted into the system.
 &lt;dhs:recordTransmission&gt;</t>
       </text>
     </comment>
     <comment ref="CO1" authorId="0" shapeId="0">
       <text>
         <t>validityTime:
-&lt;p&gt;The period of time the metadata record is valid for.&lt;/p&gt;&lt;p&gt;Must be in xsd duration form.&lt;/p&gt;&lt;p&gt;Example:&lt;ul class='no-bullets'&gt;&lt;li&gt;P1Y=Period 1 Year&lt;/li&gt;&lt;li&gt;P2M=Period 2 Months&lt;/li&gt;&lt;li&gt;P3W=Period 3 Weeks&lt;/li&gt;&lt;li&gt;P4D=Period 4 Days&lt;/li&gt;&lt;li&gt;P1Y2M=Period 1 Year &amp; 2 Months&lt;/li&gt;&lt;/ul&gt;&lt;/p&gt;
+The period of time the metadata record is valid for.
+Must be in xsd duration form.
+Example:
+P1Y=Period 1 Year
+P2M=Period 2 Months
+P3W=Period 3 Weeks
+P4D=Period 4 Days
+P1Y2M=Period 1 Year &amp; 2 Months
 &lt;dhs:validityTime&gt;</t>
       </text>
     </comment>

</xml_diff>